<commit_message>
CreateApplPage additional locators are added on 12 Feb 2024
</commit_message>
<xml_diff>
--- a/Testdata/Data.xlsx
+++ b/Testdata/Data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D2688C7-2213-4899-95BC-C016DB783E01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E0E74D3-7BA1-4B77-9F88-0F8CF6C09AD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -17,36 +17,82 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Email</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>password</t>
   </si>
   <si>
-    <t>Shiva11@gmail.com</t>
-  </si>
-  <si>
-    <t>Shiva11</t>
+    <t>username</t>
+  </si>
+  <si>
+    <t>eslsales1</t>
+  </si>
+  <si>
+    <t>themepass</t>
+  </si>
+  <si>
+    <t>PAN Card</t>
+  </si>
+  <si>
+    <t>DGNPS3255K</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Amarja</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Sonawane</t>
+  </si>
+  <si>
+    <t>Father's Name</t>
+  </si>
+  <si>
+    <t>Rajesh</t>
+  </si>
+  <si>
+    <t>Mother's Name</t>
+  </si>
+  <si>
+    <t>Anuradha</t>
+  </si>
+  <si>
+    <t>Dattatraya</t>
+  </si>
+  <si>
+    <t>Spouse</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>No. of Dependents</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Aadhar Card</t>
+  </si>
+  <si>
+    <t>440656442329</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -69,16 +115,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -95,9 +142,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -135,9 +182,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -170,26 +217,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -222,26 +252,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -415,38 +428,107 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.6328125" customWidth="1"/>
+    <col min="2" max="2" width="13.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{10A301A2-D89D-4910-87CA-B90EC1B06FFB}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -457,7 +539,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -469,7 +551,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
adding methods to File Upload and checking caption of button
</commit_message>
<xml_diff>
--- a/Testdata/Data.xlsx
+++ b/Testdata/Data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27126"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E0E74D3-7BA1-4B77-9F88-0F8CF6C09AD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5EDD657-136C-46F5-A571-2703EA1796CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4800" yWindow="2770" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>password</t>
   </si>
@@ -83,6 +83,15 @@
   </si>
   <si>
     <t>440656442329</t>
+  </si>
+  <si>
+    <t>Middle Name</t>
+  </si>
+  <si>
+    <t>Dob</t>
+  </si>
+  <si>
+    <t>19/07/1981</t>
   </si>
 </sst>
 </file>
@@ -428,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -482,50 +491,66 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
+        <v>22</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit on 20 Feb 2024
</commit_message>
<xml_diff>
--- a/Testdata/Data.xlsx
+++ b/Testdata/Data.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27126"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5EDD657-136C-46F5-A571-2703EA1796CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36ECC3E0-38F5-42C9-8E4E-EAEF78E34539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="2770" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Create_Lead" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
   <si>
     <t>password</t>
   </si>
@@ -92,6 +92,81 @@
   </si>
   <si>
     <t>19/07/1981</t>
+  </si>
+  <si>
+    <t>Customer_Type</t>
+  </si>
+  <si>
+    <t>Individual</t>
+  </si>
+  <si>
+    <t>Non-Individual</t>
+  </si>
+  <si>
+    <t>Product Type</t>
+  </si>
+  <si>
+    <t>Home Loan</t>
+  </si>
+  <si>
+    <t>Loan Against Property</t>
+  </si>
+  <si>
+    <t>Scheme</t>
+  </si>
+  <si>
+    <t>Branch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sourced By </t>
+  </si>
+  <si>
+    <t>Connector</t>
+  </si>
+  <si>
+    <t>DSA</t>
+  </si>
+  <si>
+    <t>Direct Source</t>
+  </si>
+  <si>
+    <t>Retail Finance</t>
+  </si>
+  <si>
+    <t>AHMEDABAD-7981</t>
+  </si>
+  <si>
+    <t>BANGALORE-7929</t>
+  </si>
+  <si>
+    <t>BRANCH 1-0001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source Name </t>
+  </si>
+  <si>
+    <t>Connector-Test1</t>
+  </si>
+  <si>
+    <t>DSA-Test1</t>
+  </si>
+  <si>
+    <t>Cold Call</t>
+  </si>
+  <si>
+    <t>Marketing Campaign</t>
+  </si>
+  <si>
+    <t>Customer Referal</t>
+  </si>
+  <si>
+    <t>Employee Referal</t>
+  </si>
+  <si>
+    <t>Social Media</t>
+  </si>
+  <si>
+    <t>Builder</t>
   </si>
 </sst>
 </file>
@@ -439,8 +514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -560,13 +635,170 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:XFD27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="15.1796875" customWidth="1"/>
+    <col min="2" max="2" width="19.7265625" customWidth="1"/>
+    <col min="3" max="3" width="13.54296875" customWidth="1"/>
+    <col min="4" max="4" width="15.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B5" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B13" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B14" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B31" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B32" s="1"/>
+      <c r="D32" s="1"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B33" s="1"/>
+      <c r="D33" s="1"/>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B34" s="1"/>
+      <c r="D34" s="1"/>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B35" s="1"/>
+      <c r="D35" s="1"/>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B36" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="D37" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="D38" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="D39" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="D40" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="D41" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
created new data file and created new flows 1 for accept and 1 for reject on 22 Feb 2024
</commit_message>
<xml_diff>
--- a/Testdata/Data.xlsx
+++ b/Testdata/Data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27126"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36ECC3E0-38F5-42C9-8E4E-EAEF78E34539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C0A3CE6-4246-4695-AFDA-7B90CD0F9ABD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="94">
   <si>
     <t>password</t>
   </si>
@@ -100,18 +100,12 @@
     <t>Individual</t>
   </si>
   <si>
-    <t>Non-Individual</t>
-  </si>
-  <si>
     <t>Product Type</t>
   </si>
   <si>
     <t>Home Loan</t>
   </si>
   <si>
-    <t>Loan Against Property</t>
-  </si>
-  <si>
     <t>Scheme</t>
   </si>
   <si>
@@ -124,49 +118,187 @@
     <t>Connector</t>
   </si>
   <si>
-    <t>DSA</t>
-  </si>
-  <si>
-    <t>Direct Source</t>
-  </si>
-  <si>
     <t>Retail Finance</t>
   </si>
   <si>
     <t>AHMEDABAD-7981</t>
   </si>
   <si>
+    <t xml:space="preserve">Source Name </t>
+  </si>
+  <si>
+    <t>Connector-Test1</t>
+  </si>
+  <si>
+    <t>Amt Req</t>
+  </si>
+  <si>
+    <t>5000000</t>
+  </si>
+  <si>
+    <t>PAN</t>
+  </si>
+  <si>
+    <t>DOB</t>
+  </si>
+  <si>
+    <t>MobileNo</t>
+  </si>
+  <si>
+    <t>9850865458</t>
+  </si>
+  <si>
+    <t>STD</t>
+  </si>
+  <si>
+    <t>022</t>
+  </si>
+  <si>
+    <t>Landline</t>
+  </si>
+  <si>
+    <t>65016500</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Addr1</t>
+  </si>
+  <si>
+    <t>Addr2</t>
+  </si>
+  <si>
+    <t>Pincode</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Next Commencement Date</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Created for Testing Purpose</t>
+  </si>
+  <si>
+    <t>Lead created</t>
+  </si>
+  <si>
+    <t>abc@gmail.com</t>
+  </si>
+  <si>
+    <t>Mumbai</t>
+  </si>
+  <si>
+    <t>Maharashtra</t>
+  </si>
+  <si>
+    <t>Dynasty Business Park</t>
+  </si>
+  <si>
+    <t>Andheri- Kurla Road</t>
+  </si>
+  <si>
+    <t>400059</t>
+  </si>
+  <si>
+    <t>COLD</t>
+  </si>
+  <si>
+    <t>PENDING</t>
+  </si>
+  <si>
+    <t>19/07/1990</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>15/04/2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lead status </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wait </t>
+  </si>
+  <si>
+    <t>Particulars</t>
+  </si>
+  <si>
+    <t>Lead 1</t>
+  </si>
+  <si>
+    <t>Lead 2</t>
+  </si>
+  <si>
+    <t>Lead 3</t>
+  </si>
+  <si>
+    <t>LeadId</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>convert</t>
+  </si>
+  <si>
     <t>BANGALORE-7929</t>
   </si>
   <si>
-    <t>BRANCH 1-0001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Source Name </t>
-  </si>
-  <si>
-    <t>Connector-Test1</t>
-  </si>
-  <si>
-    <t>DSA-Test1</t>
-  </si>
-  <si>
-    <t>Cold Call</t>
-  </si>
-  <si>
-    <t>Marketing Campaign</t>
-  </si>
-  <si>
-    <t>Customer Referal</t>
-  </si>
-  <si>
-    <t>Employee Referal</t>
-  </si>
-  <si>
-    <t>Social Media</t>
-  </si>
-  <si>
-    <t>Builder</t>
+    <t>AZUPS3267K</t>
+  </si>
+  <si>
+    <t>Rima</t>
+  </si>
+  <si>
+    <t>Karmakar</t>
+  </si>
+  <si>
+    <t>22/06/1992</t>
+  </si>
+  <si>
+    <t>65016501</t>
+  </si>
+  <si>
+    <t>xyz@gmail.com</t>
+  </si>
+  <si>
+    <t>BKC</t>
+  </si>
+  <si>
+    <t>Bandra-Kurla Road</t>
+  </si>
+  <si>
+    <t>20/05/2024</t>
+  </si>
+  <si>
+    <t>400058</t>
+  </si>
+  <si>
+    <t>9004263223</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>10000000</t>
+  </si>
+  <si>
+    <t>Lead Created for reject</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Created for Rejection </t>
   </si>
 </sst>
 </file>
@@ -182,12 +314,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -202,12 +340,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -515,7 +671,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A8" sqref="A8:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -635,165 +791,360 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:T30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:XFD27"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15.1796875" customWidth="1"/>
-    <col min="2" max="2" width="19.7265625" customWidth="1"/>
-    <col min="3" max="3" width="13.54296875" customWidth="1"/>
-    <col min="4" max="4" width="15.7265625" customWidth="1"/>
+    <col min="2" max="2" width="24.26953125" customWidth="1"/>
+    <col min="3" max="3" width="24.08984375" customWidth="1"/>
+    <col min="4" max="4" width="13.54296875" style="7" customWidth="1"/>
+    <col min="5" max="5" width="16.08984375" customWidth="1"/>
+    <col min="6" max="6" width="14.81640625" customWidth="1"/>
+    <col min="7" max="7" width="10.1796875" customWidth="1"/>
+    <col min="8" max="8" width="10" customWidth="1"/>
+    <col min="9" max="9" width="10.54296875" customWidth="1"/>
+    <col min="11" max="11" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.36328125" customWidth="1"/>
+    <col min="15" max="15" width="20.36328125" customWidth="1"/>
+    <col min="16" max="16" width="18.26953125" customWidth="1"/>
+    <col min="19" max="19" width="12.6328125" customWidth="1"/>
+    <col min="20" max="20" width="10.1796875" customWidth="1"/>
+    <col min="21" max="21" width="18.36328125" customWidth="1"/>
+    <col min="22" max="22" width="11.6328125" customWidth="1"/>
+    <col min="23" max="23" width="24.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" s="6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B2" t="s">
+      <c r="C2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="B5" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>32</v>
+      <c r="B9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A10" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A13" s="5" t="s">
+        <v>40</v>
+      </c>
       <c r="B13" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+        <v>66</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A14" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="B14" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" s="1" t="s">
-        <v>33</v>
+        <v>67</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A15" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A16" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A25" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" s="5" t="s">
+        <v>54</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B31" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B32" s="1"/>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B33" s="1"/>
-      <c r="D33" s="1"/>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B34" s="1"/>
-      <c r="D34" s="1"/>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B35" s="1"/>
-      <c r="D35" s="1"/>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B36" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="D37" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="D38" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="D39" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="D40" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="D41" s="1" t="s">
-        <v>49</v>
+        <v>57</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>76</v>
+      </c>
+      <c r="B30" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -804,12 +1155,133 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:S1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:19" ht="58" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J2" t="s">
+        <v>58</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>